<commit_message>
Thêm bảng phân công công việc
</commit_message>
<xml_diff>
--- a/bangphancongcv.xlsx
+++ b/bangphancongcv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoa2\OneDrive\Máy tính\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khoa2\OneDrive\Máy tính\BC32E_LeNguyenTheKhoa_TranVanKhang_Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC74283-7215-4FF3-B1FE-D3ECEB095C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F1AE89-0D93-4312-B07A-F6614BF8DB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{68DE72E1-56BD-4F15-943C-C9D1E7017478}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Backtotop</t>
   </si>
   <si>
-    <t>Start Builds</t>
-  </si>
-  <si>
     <t>Finish Build</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Host web</t>
+  </si>
+  <si>
+    <t>Start Build</t>
   </si>
 </sst>
 </file>
@@ -198,27 +198,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1322,14 +1327,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>457200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="203200" cy="203200"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>622300</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -1338,7 +1348,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D49832BC-E00E-4364-8C40-1FB10E92AA18}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1378,20 +1388,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>457200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="203200" cy="203200"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>622300</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -1400,7 +1415,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D07C1538-C142-46FF-AB86-5542AAB3B42E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1440,20 +1455,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>133350</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="203200" cy="203200"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>336550</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
@@ -1462,7 +1482,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A4647E3-8BBC-4E4C-AB80-8E5577122BCF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1502,7 +1522,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1529,7 +1549,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C731A1B9-35E1-6E4D-65C4-A18B000BF730}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1876,320 +1896,320 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>44709</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>44710</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
+      <c r="E2" s="3"/>
+      <c r="F2" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>44709</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>44710</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
+      <c r="E3" s="3"/>
+      <c r="F3" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>44709</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>44710</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
+      <c r="E4" s="3"/>
+      <c r="F4" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>44710</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>44713</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
+      <c r="E5" s="3"/>
+      <c r="F5" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>44710</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>44713</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
+      <c r="E6" s="3"/>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>44710</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>44713</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
+      <c r="E7" s="3"/>
+      <c r="F7" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>44711</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>44719</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="2" t="s">
-        <v>22</v>
+      <c r="E8" s="3"/>
+      <c r="F8" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>44713</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>44719</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
+      <c r="E9" s="3"/>
+      <c r="F9" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>44713</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>44719</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="2" t="s">
-        <v>22</v>
+      <c r="E10" s="3"/>
+      <c r="F10" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>44713</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>44719</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>1</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>44713</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>44719</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="2" t="s">
-        <v>22</v>
+      <c r="E12" s="3"/>
+      <c r="F12" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>44713</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>44719</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>1</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="2" t="s">
-        <v>22</v>
+      <c r="E13" s="3"/>
+      <c r="F13" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>44717</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>44717</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
+      <c r="E14" s="3"/>
+      <c r="F14" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>44722</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44722</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="B15" s="3">
-        <v>44722</v>
-      </c>
-      <c r="C15" s="3">
-        <v>44722</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44722</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44722</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" s="3">
-        <v>44722</v>
-      </c>
-      <c r="C16" s="3">
-        <v>44722</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
         <v>44722</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>44722</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>